<commit_message>
update: att product started
</commit_message>
<xml_diff>
--- a/produtos.xlsx
+++ b/produtos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,11 +474,6 @@
           <t>Estoque</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 8</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -511,7 +506,6 @@
       <c r="H2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -544,7 +538,6 @@
       <c r="H3" t="n">
         <v>0</v>
       </c>
-      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -577,7 +570,6 @@
       <c r="H4" t="n">
         <v>0</v>
       </c>
-      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -610,7 +602,6 @@
       <c r="H5" t="n">
         <v>12</v>
       </c>
-      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -643,7 +634,6 @@
       <c r="H6" t="n">
         <v>14</v>
       </c>
-      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -676,7 +666,6 @@
       <c r="H7" t="n">
         <v>7</v>
       </c>
-      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -709,7 +698,6 @@
       <c r="H8" t="n">
         <v>0</v>
       </c>
-      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -742,7 +730,6 @@
       <c r="H9" t="n">
         <v>0</v>
       </c>
-      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -775,7 +762,6 @@
       <c r="H10" t="n">
         <v>0</v>
       </c>
-      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -808,7 +794,6 @@
       <c r="H11" t="n">
         <v>-2</v>
       </c>
-      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -841,36 +826,44 @@
       <c r="H12" t="n">
         <v>0</v>
       </c>
-      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>OI</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Tenis</t>
+          <t>Oi</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Novo</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F13" t="n">
-        <v>20000</v>
+          <t>Oi</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>112</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
       </c>
       <c r="G13" t="n">
-        <v>19000</v>
-      </c>
-      <c r="H13" t="n">
-        <v>20</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Tenis Nike</t>
+        <v>22</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>

</xml_diff>